<commit_message>
add: unit test for banner; fix: refix import product template
</commit_message>
<xml_diff>
--- a/app/order-api/public/templates/excel/import-products.xlsx
+++ b/app/order-api/public/templates/excel/import-products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Order\order\app\order-api\public\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E2F05D-5C12-4AC2-868B-CC31781627C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68828A6-83BF-49BC-B42A-8AEC66BED78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="-15195" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import sản phẩm" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Stt</t>
   </si>
   <si>
     <t>Tên sản phẩm</t>
-  </si>
-  <si>
-    <t>Nhóm hàng</t>
   </si>
   <si>
     <t>Mô tả</t>
@@ -56,6 +53,36 @@
   </si>
   <si>
     <t>Giá kích thước 3</t>
+  </si>
+  <si>
+    <t>Nhóm hàng (Đồ ăn, nước uống,…)</t>
+  </si>
+  <si>
+    <t>Cà phê</t>
+  </si>
+  <si>
+    <t>Nước uống</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Bún bò</t>
+  </si>
+  <si>
+    <t>Đồ ăn</t>
+  </si>
+  <si>
+    <t>Cà phê thượng hạng</t>
+  </si>
+  <si>
+    <t>Thịt bò tuyển chọn</t>
   </si>
 </sst>
 </file>
@@ -382,7 +409,7 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -403,34 +430,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -450,19 +477,39 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+    <row r="2" spans="1:29" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4">
+        <v>25000</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4">
+        <v>30000</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -481,19 +528,39 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+    <row r="3" spans="1:29" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4">
+        <v>40000</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4">
+        <v>50000</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4">
+        <v>60000</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>

</xml_diff>